<commit_message>
Goodbye PerfectIP, Hello MCLP
</commit_message>
<xml_diff>
--- a/MultipleIP/9x9/compare2.xlsx
+++ b/MultipleIP/9x9/compare2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="92">
   <si>
     <t>P(Arrival)</t>
   </si>
@@ -62,58 +62,55 @@
     <t>13.0</t>
   </si>
   <si>
-    <t>83.5</t>
+    <t>83.9</t>
+  </si>
+  <si>
+    <t>13.7</t>
+  </si>
+  <si>
+    <t>0.42</t>
+  </si>
+  <si>
+    <t>0.38</t>
+  </si>
+  <si>
+    <t>95.7</t>
+  </si>
+  <si>
+    <t>14.7</t>
+  </si>
+  <si>
+    <t>95.2</t>
+  </si>
+  <si>
+    <t>14.1</t>
+  </si>
+  <si>
+    <t>96.3</t>
+  </si>
+  <si>
+    <t>15.5</t>
+  </si>
+  <si>
+    <t>0.47</t>
+  </si>
+  <si>
+    <t>0.43</t>
+  </si>
+  <si>
+    <t>93.0</t>
+  </si>
+  <si>
+    <t>107.4</t>
+  </si>
+  <si>
+    <t>15.6</t>
+  </si>
+  <si>
+    <t>105.1</t>
   </si>
   <si>
     <t>13.1</t>
-  </si>
-  <si>
-    <t>83.9</t>
-  </si>
-  <si>
-    <t>13.7</t>
-  </si>
-  <si>
-    <t>0.42</t>
-  </si>
-  <si>
-    <t>0.38</t>
-  </si>
-  <si>
-    <t>95.7</t>
-  </si>
-  <si>
-    <t>14.7</t>
-  </si>
-  <si>
-    <t>95.2</t>
-  </si>
-  <si>
-    <t>14.1</t>
-  </si>
-  <si>
-    <t>96.3</t>
-  </si>
-  <si>
-    <t>15.5</t>
-  </si>
-  <si>
-    <t>0.47</t>
-  </si>
-  <si>
-    <t>0.43</t>
-  </si>
-  <si>
-    <t>93.0</t>
-  </si>
-  <si>
-    <t>107.4</t>
-  </si>
-  <si>
-    <t>15.6</t>
-  </si>
-  <si>
-    <t>105.1</t>
   </si>
   <si>
     <t>108.1</t>
@@ -300,8 +297,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -388,7 +386,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -412,12 +410,16 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="10.5561224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="12" min="9" style="0" width="10.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -481,7 +483,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>0.06</v>
       </c>
@@ -507,358 +509,358 @@
         <v>14</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="2" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="3" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="K5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="3" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="3" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="L7" s="3" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="E10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="L9" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="F11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="F12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="I12" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="I12" s="3" t="s">
+      <c r="J12" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="K12" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>54</v>
+      <c r="L12" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -875,7 +877,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.3" right="0.3" top="0.609722222222222" bottom="0.370138888888889" header="0.1" footer="0.1"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;P</oddHeader>
     <oddFooter>&amp;C&amp;F</oddFooter>

</xml_diff>